<commit_message>
What the fuck do you think I changed?
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan\Desktop\Lunar Hopper\Organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jt6g15\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{4E083F9A-2823-4C42-AF8E-D45D00D65241}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="139">
   <si>
     <t>Lunar Hopper Inventory</t>
   </si>
@@ -438,12 +438,15 @@
   </si>
   <si>
     <t>B2G</t>
+  </si>
+  <si>
+    <t>31/10/2017 - With Bhagyesh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -788,11 +791,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8335353D-7F21-4182-9C75-44D9A9761D12}">
-  <dimension ref="C3:F97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,6 +803,7 @@
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
@@ -954,7 +958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>21</v>
       </c>
@@ -965,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>22</v>
       </c>
@@ -976,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>24</v>
       </c>
@@ -987,7 +991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>25</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>26</v>
       </c>
@@ -1012,7 +1016,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>29</v>
       </c>
@@ -1023,7 +1027,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>30</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>32</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>34</v>
       </c>
@@ -1059,7 +1063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>37</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>38</v>
       </c>
@@ -1081,7 +1085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +1096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>40</v>
       </c>
@@ -1103,7 +1107,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>41</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>17</v>
       </c>
@@ -1127,8 +1131,11 @@
       <c r="F31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>45</v>
       </c>

</xml_diff>